<commit_message>
Updated article on Cambridge seat odds
</commit_message>
<xml_diff>
--- a/cambridge/elections/2015/ladbrokes/Ladbrokes data.xlsx
+++ b/cambridge/elections/2015/ladbrokes/Ladbrokes data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>LD</t>
   </si>
@@ -30,24 +30,34 @@
     <t>Grn</t>
   </si>
   <si>
-    <t>Jan 2013</t>
-  </si>
-  <si>
-    <t>Dec 2013</t>
-  </si>
-  <si>
     <t>Lib Dem</t>
   </si>
   <si>
     <t>Green</t>
+  </si>
+  <si>
+    <t>Fractional odds</t>
+  </si>
+  <si>
+    <t>Decimal odds</t>
+  </si>
+  <si>
+    <t>&lt;- this is the overround</t>
+  </si>
+  <si>
+    <t>Reciprocal</t>
+  </si>
+  <si>
+    <t>Implied probability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="mmm\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -89,10 +99,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +167,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$14</c:f>
+              <c:f>Sheet1!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -186,30 +196,37 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$15:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\ yyyy</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Jan 2013</c:v>
+                  <c:v>41275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Dec 2013</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>41609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$16</c:f>
+              <c:f>Sheet1!$B$21:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.56220472440944891</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.52055993000874889</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50552251486830935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -221,7 +238,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$14</c:f>
+              <c:f>Sheet1!$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -250,30 +267,37 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$15:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\ yyyy</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Jan 2013</c:v>
+                  <c:v>41275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Dec 2013</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>41609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$C$16</c:f>
+              <c:f>Sheet1!$C$21:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.37480314960629924</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.41644794400699908</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43330501274426508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -285,7 +309,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$14</c:f>
+              <c:f>Sheet1!$D$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -314,30 +338,37 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$15:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\ yyyy</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Jan 2013</c:v>
+                  <c:v>41275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Dec 2013</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>41609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$15:$D$16</c:f>
+              <c:f>Sheet1!$D$21:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4.4619422572178477E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.4619422572178477E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.333050127442651E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,7 +380,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$14</c:f>
+              <c:f>Sheet1!$E$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -378,30 +409,37 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$15:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\ yyyy</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Jan 2013</c:v>
+                  <c:v>41275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Dec 2013</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>41609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$15:$E$16</c:f>
+              <c:f>Sheet1!$E$21:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.8372703412073491E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.8372703412073491E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7841971112999153E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,28 +456,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93129728"/>
-        <c:axId val="93463296"/>
+        <c:axId val="136260992"/>
+        <c:axId val="136287744"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="93129728"/>
+      <c:dateAx>
+        <c:axId val="136260992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\ yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93463296"/>
+        <c:crossAx val="136287744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="93463296"/>
+        <c:axId val="136287744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -450,7 +488,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93129728"/>
+        <c:crossAx val="136260992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -471,16 +509,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>338136</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>33336</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -497,6 +535,102 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="314325" y="4857750"/>
+          <a:ext cx="4305300" cy="2705100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Here's how to turn a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> set of odds into implied probability:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>1) Convert fractional (a/b) odds into decimal odds by calculating 1+a/b</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>2) Take the reciprocal (1/x) of each number, giving an implied probability - convert this to a percentage</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>3) Add them all up - you'll get a bit more than 100%. This is because there's an "overround" built in to the odds to give the bookie a profit</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>4) Divide each number by the overround to get a set of probabilities that add up to 100</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -789,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,115 +935,124 @@
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>6</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>4</v>
-      </c>
-      <c r="D1">
-        <f>1+B1/C1</f>
-        <v>2.5</v>
-      </c>
-      <c r="E1">
-        <f>1/D1</f>
-        <v>0.4</v>
-      </c>
-      <c r="F1" s="1">
-        <f>E1/E$5</f>
-        <v>0.37480314960629924</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
       </c>
       <c r="D2">
         <f>1+B2/C2</f>
-        <v>1.6666666666666665</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <f>1/D2</f>
-        <v>0.60000000000000009</v>
+        <v>0.4</v>
       </c>
       <c r="F2" s="1">
-        <f>E2/E$5</f>
-        <v>0.56220472440944891</v>
-      </c>
-      <c r="J2" s="5">
-        <v>42131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <f>E2/E$6</f>
+        <v>0.37480314960629924</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <f>1+B3/C3</f>
-        <v>21</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="E3">
         <f>1/D3</f>
-        <v>4.7619047619047616E-2</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="F3" s="1">
-        <f>E3/E$5</f>
-        <v>4.4619422572178477E-2</v>
-      </c>
-      <c r="J3" s="5">
-        <v>41629</v>
-      </c>
-      <c r="K3">
-        <f>J2-J3</f>
-        <v>502</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <f>E3/E$6</f>
+        <v>0.56220472440944891</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
         <f>1+B4/C4</f>
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <f>1/D4</f>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4/E$6</f>
+        <v>4.4619422572178477E-2</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f>1+B5/C5</f>
+        <v>51</v>
+      </c>
+      <c r="E5">
+        <f>1/D5</f>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="F4" s="1">
-        <f>E4/E$5</f>
+      <c r="F5" s="1">
+        <f>E5/E$6</f>
         <v>1.8372703412073491E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <f>SUM(E1:E4)</f>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>SUM(E2:E5)</f>
         <v>1.0672268907563025</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -932,7 +1075,7 @@
         <v>0.41644794400699908</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -955,7 +1098,7 @@
         <v>0.52055993000874889</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -978,7 +1121,7 @@
         <v>4.4619422572178477E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1001,71 +1144,203 @@
         <v>1.8372703412073491E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E12">
         <f>SUM(E8:E11)</f>
         <v>1.0672268907563025</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <f>1+B14/C14</f>
+        <v>2.1</v>
+      </c>
+      <c r="E14">
+        <f>1/D14</f>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14/E$18</f>
+        <v>0.43330501274426508</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <f>1+B15/C15</f>
+        <v>1.8</v>
+      </c>
+      <c r="E15">
+        <f>1/D15</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15/E$18</f>
+        <v>0.50552251486830935</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f>1+B16/C16</f>
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <f>1/D16</f>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16/E$18</f>
+        <v>4.333050127442651E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>1+B17/C17</f>
+        <v>51</v>
+      </c>
+      <c r="E17">
+        <f>1/D17</f>
+        <v>1.9607843137254902E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17/E$18</f>
+        <v>1.7841971112999153E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f>SUM(E14:E17)</f>
+        <v>1.0989729225023341</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="4">
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>41275</v>
+      </c>
+      <c r="B21" s="2">
+        <f>F3</f>
+        <v>0.56220472440944891</v>
+      </c>
+      <c r="C21" s="2">
         <f>F2</f>
-        <v>0.56220472440944891</v>
-      </c>
-      <c r="C15" s="4">
-        <f>F1</f>
         <v>0.37480314960629924</v>
       </c>
-      <c r="D15" s="4">
-        <f>F3</f>
+      <c r="D21" s="2">
+        <f>F4</f>
         <v>4.4619422572178477E-2</v>
       </c>
-      <c r="E15" s="4">
-        <f>F4</f>
+      <c r="E21" s="2">
+        <f>F5</f>
         <v>1.8372703412073491E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="G21" s="2">
+        <f>SUM(B21:E21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>41609</v>
+      </c>
+      <c r="B22" s="2">
         <f>F9</f>
         <v>0.52055993000874889</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C22" s="2">
         <f>F8</f>
         <v>0.41644794400699908</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D22" s="2">
         <f>F10</f>
         <v>4.4619422572178477E-2</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E22" s="2">
         <f>F11</f>
         <v>1.8372703412073491E-2</v>
       </c>
+      <c r="G22" s="2">
+        <f>SUM(B22:E22)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>41699</v>
+      </c>
+      <c r="B23" s="2">
+        <f>F15</f>
+        <v>0.50552251486830935</v>
+      </c>
+      <c r="C23" s="2">
+        <f>F14</f>
+        <v>0.43330501274426508</v>
+      </c>
+      <c r="D23" s="2">
+        <f>F16</f>
+        <v>4.333050127442651E-2</v>
+      </c>
+      <c r="E23" s="2">
+        <f>F17</f>
+        <v>1.7841971112999153E-2</v>
+      </c>
+      <c r="G23" s="2">
+        <f>SUM(B23:E23)</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>